<commit_message>
added has posted and legal_entites
</commit_message>
<xml_diff>
--- a/data/vocab-tagged.xlsx
+++ b/data/vocab-tagged.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/okhrimchuk/business/citi/asr/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7E5B4C-C9D7-AD4A-84BB-42F96C75A0F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E78E167-ECCD-CD49-91EC-61A124C416DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{E61FADE1-B4E3-634F-BA00-D3AA603E5BA7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>select</t>
   </si>
@@ -60,9 +60,6 @@
     <t>usmuni</t>
   </si>
   <si>
-    <t>assets</t>
-  </si>
-  <si>
     <t>clause_operators</t>
   </si>
   <si>
@@ -70,6 +67,21 @@
   </si>
   <si>
     <t>initial_operators</t>
+  </si>
+  <si>
+    <t>collateral</t>
+  </si>
+  <si>
+    <t>legal_entity</t>
+  </si>
+  <si>
+    <t>cgmi</t>
+  </si>
+  <si>
+    <t>cgml</t>
+  </si>
+  <si>
+    <t>cgma</t>
   </si>
 </sst>
 </file>
@@ -421,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE653D3-E0F4-CF45-AD78-90B643C249C2}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -434,21 +446,24 @@
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
+      <c r="E1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -461,8 +476,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -475,16 +493,25 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
       </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
new query generation algo
</commit_message>
<xml_diff>
--- a/data/vocab-tagged.xlsx
+++ b/data/vocab-tagged.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/okhrimchuk/business/citi/asr/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/okhrimchuk/business/citi/asr/ASR_Citi/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E78E167-ECCD-CD49-91EC-61A124C416DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CACB2EB-11A5-1A4C-9039-AC8F60F2ED08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="15000" xr2:uid="{E61FADE1-B4E3-634F-BA00-D3AA603E5BA7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>select</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>cgma</t>
+  </si>
+  <si>
+    <t>intersection_operators</t>
   </si>
 </sst>
 </file>
@@ -433,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AE653D3-E0F4-CF45-AD78-90B643C249C2}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,73 +449,73 @@
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>13</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>